<commit_message>
added band area parameters, updated denoise routine
</commit_message>
<xml_diff>
--- a/hypyrameter/ImageCubeParameters/browseDefinitions.xlsx
+++ b/hypyrameter/ImageCubeParameters/browseDefinitions.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillms1/Documents/Work/RAVEN/HyPyRameter/HyPyRameter/hypyrameter/ImageCubeParameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D175DF-4AA7-D24C-9C84-0193630EB775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529D2BD3-1CFE-264D-AA2F-237381189997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{6CF0468C-FC83-8C46-915E-64DBB71650C8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="10000" windowHeight="16940" xr2:uid="{6CF0468C-FC83-8C46-915E-64DBB71650C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$15</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>BrowseProduct</t>
   </si>
@@ -190,6 +190,18 @@
   </si>
   <si>
     <t>GINDEX</t>
+  </si>
+  <si>
+    <t>HY3</t>
+  </si>
+  <si>
+    <t>BA1200</t>
+  </si>
+  <si>
+    <t>BA1450</t>
+  </si>
+  <si>
+    <t>BA1900</t>
   </si>
 </sst>
 </file>
@@ -541,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57500815-3920-3043-86A5-AE204CD247BD}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,113 +652,127 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added point parameter example and USGS library parameter values for reference
</commit_message>
<xml_diff>
--- a/hypyrameter/ImageCubeParameters/browseDefinitions.xlsx
+++ b/hypyrameter/ImageCubeParameters/browseDefinitions.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillms1/Documents/Work/RAVEN/HyPyRameter/HyPyRameter/hypyrameter/ImageCubeParameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipsm/Documents/Software/HyPyRameter/hypyrameter/ImageCubeParameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529D2BD3-1CFE-264D-AA2F-237381189997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38081E44-88EF-6B4A-8EB0-85A407222EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="10000" windowHeight="16940" xr2:uid="{6CF0468C-FC83-8C46-915E-64DBB71650C8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="16560" windowHeight="16940" xr2:uid="{6CF0468C-FC83-8C46-915E-64DBB71650C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$17</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>BrowseProduct</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>BA1900</t>
+  </si>
+  <si>
+    <t>MAF2</t>
+  </si>
+  <si>
+    <t>BIO</t>
+  </si>
+  <si>
+    <t>D700</t>
   </si>
 </sst>
 </file>
@@ -553,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57500815-3920-3043-86A5-AE204CD247BD}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,141 +647,169 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
         <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
udpdated parameter library and browse product definitions
</commit_message>
<xml_diff>
--- a/hypyrameter/ImageCubeParameters/browseDefinitions.xlsx
+++ b/hypyrameter/ImageCubeParameters/browseDefinitions.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipsm/Documents/Software/HyPyRameter/hypyrameter/ImageCubeParameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38081E44-88EF-6B4A-8EB0-85A407222EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CCB349-5F62-D442-B1C6-FA87601B9487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="16560" windowHeight="16940" xr2:uid="{6CF0468C-FC83-8C46-915E-64DBB71650C8}"/>
+    <workbookView xWindow="3360" yWindow="760" windowWidth="16560" windowHeight="16940" xr2:uid="{6CF0468C-FC83-8C46-915E-64DBB71650C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$19</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>BrowseProduct</t>
   </si>
@@ -102,9 +102,6 @@
     <t>HYS</t>
   </si>
   <si>
-    <t>HY2</t>
-  </si>
-  <si>
     <t>SED</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
     <t>GINDEX</t>
   </si>
   <si>
-    <t>HY3</t>
-  </si>
-  <si>
     <t>BA1200</t>
   </si>
   <si>
@@ -204,13 +198,37 @@
     <t>BA1900</t>
   </si>
   <si>
-    <t>MAF2</t>
-  </si>
-  <si>
     <t>BIO</t>
   </si>
   <si>
     <t>D700</t>
+  </si>
+  <si>
+    <t>PLG</t>
+  </si>
+  <si>
+    <t>BD1300</t>
+  </si>
+  <si>
+    <t>RPEAK1</t>
+  </si>
+  <si>
+    <t>HYD2</t>
+  </si>
+  <si>
+    <t>HYD3</t>
+  </si>
+  <si>
+    <t>FM3</t>
+  </si>
+  <si>
+    <t>BD905</t>
+  </si>
+  <si>
+    <t>SUL</t>
+  </si>
+  <si>
+    <t>BD2265</t>
   </si>
 </sst>
 </file>
@@ -562,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57500815-3920-3043-86A5-AE204CD247BD}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,156 +609,156 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -748,13 +766,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -762,13 +780,13 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
         <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -776,44 +794,75 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D19" t="s">
         <v>29</v>
       </c>
-      <c r="D17" t="s">
-        <v>30</v>
-      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D19">
+    <sortCondition ref="A2:A19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>